<commit_message>
Added parsing of write-results argument to decide whether to write results, and where to. Added helper function to assert library to avoid having to check if results should be written from every assert function. Added example run command to readme
</commit_message>
<xml_diff>
--- a/Windows.xlsx
+++ b/Windows.xlsx
@@ -336,10 +336,10 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.43"/>

</xml_diff>

<commit_message>
Only init RegressionSheet if writting to it
</commit_message>
<xml_diff>
--- a/Windows.xlsx
+++ b/Windows.xlsx
@@ -336,10 +336,10 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.43"/>

</xml_diff>

<commit_message>
Renamed RegressionSheet to RegressionSheetWriter. Removed of success from main
</commit_message>
<xml_diff>
--- a/Windows.xlsx
+++ b/Windows.xlsx
@@ -336,10 +336,10 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.43"/>

</xml_diff>